<commit_message>
Addressing duplicate exetainer codes. Need to hardcode results in duplicated_exetainers.xlsx in readGC.R. In development
</commit_message>
<xml_diff>
--- a/SuRGE_Sharepoint/data/R10/CH4_287_Owyhee/dataSheets/surgeData287.xlsx
+++ b/SuRGE_Sharepoint/data/R10/CH4_287_Owyhee/dataSheets/surgeData287.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa.sharepoint.com/sites/SuRGE/Shared Documents/data/R10/CH4_287_owyhee/dataSheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/beaulieu_jake_epa_gov/Documents/gitRepository/SuRGE/SuRGE_Sharepoint/data/R10/CH4_287_Owyhee/dataSheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="995" documentId="8_{574317AD-36CA-42B2-83FE-C04BF0299D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{935C0C96-9C56-4E74-A164-009F02726630}"/>
+  <xr:revisionPtr revIDLastSave="997" documentId="8_{574317AD-36CA-42B2-83FE-C04BF0299D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BDF1CCB-0905-4C76-9D7E-E52BE615471E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9000" yWindow="3504" windowWidth="34560" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -1344,9 +1344,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1384,7 +1384,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1490,7 +1490,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1632,7 +1632,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1643,79 +1643,79 @@
   <dimension ref="A1:BP18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AE1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AE15" sqref="AE15"/>
+      <pane xSplit="2" topLeftCell="AQ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BL16" sqref="BL16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="9" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="4.88671875" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="6" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="18" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="8" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="11" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="10" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="14" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="62" max="64" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="65" max="66" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="62" max="64" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="65" max="66" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="22.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
         <v>54</v>
       </c>
@@ -1797,7 +1797,7 @@
       <c r="BO1" s="30"/>
       <c r="BP1" s="30"/>
     </row>
-    <row r="2" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>173</v>
       </c>
@@ -2013,15 +2013,6 @@
       <c r="C3" t="s">
         <v>174</v>
       </c>
-      <c r="BJ3" t="s">
-        <v>191</v>
-      </c>
-      <c r="BK3" t="s">
-        <v>192</v>
-      </c>
-      <c r="BL3" t="s">
-        <v>193</v>
-      </c>
       <c r="BM3">
         <v>2</v>
       </c>
@@ -2035,7 +2026,7 @@
         <v>0.77638888888888891</v>
       </c>
     </row>
-    <row r="4" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
         <v>173</v>
       </c>
@@ -2138,8 +2129,17 @@
       <c r="BI4" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="5" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="BJ4" t="s">
+        <v>191</v>
+      </c>
+      <c r="BK4" t="s">
+        <v>192</v>
+      </c>
+      <c r="BL4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
         <v>173</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
         <v>173</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="7" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
         <v>173</v>
       </c>
@@ -2460,7 +2460,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="8" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A8" s="25" t="s">
         <v>173</v>
       </c>
@@ -2564,7 +2564,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="9" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A9" s="25" t="s">
         <v>173</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="10" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A10" s="25" t="s">
         <v>173</v>
       </c>
@@ -2790,7 +2790,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="11" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A11" s="25" t="s">
         <v>173</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="12" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
         <v>173</v>
       </c>
@@ -2998,7 +2998,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="13" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
         <v>173</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="14" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
         <v>173</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="15" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A15" s="25" t="s">
         <v>173</v>
       </c>
@@ -3313,7 +3313,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="16" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
         <v>173</v>
       </c>
@@ -3417,7 +3417,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="17" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:61" x14ac:dyDescent="0.3">
       <c r="A17" s="25" t="s">
         <v>173</v>
       </c>
@@ -3524,7 +3524,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="18" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:61" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
         <v>173</v>
       </c>
@@ -3654,14 +3654,14 @@
       <selection activeCell="A68" sqref="A68:A69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="116.7109375" customWidth="1"/>
-    <col min="3" max="3" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="116.6640625" customWidth="1"/>
+    <col min="3" max="3" width="49.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>135</v>
       </c>
@@ -3672,7 +3672,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3683,7 +3683,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3694,7 +3694,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>2</v>
       </c>
@@ -3705,7 +3705,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -3716,7 +3716,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -3738,7 +3738,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -3749,7 +3749,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -3760,7 +3760,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -3771,7 +3771,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -3782,7 +3782,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -3793,7 +3793,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -3804,7 +3804,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -3812,7 +3812,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -3823,7 +3823,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -3831,7 +3831,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -3842,7 +3842,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -3861,7 +3861,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -3872,7 +3872,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -3883,7 +3883,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -3894,7 +3894,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -3916,7 +3916,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -3960,7 +3960,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -3971,7 +3971,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>148</v>
       </c>
@@ -3982,7 +3982,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -3993,7 +3993,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -4001,7 +4001,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -4009,7 +4009,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -4017,7 +4017,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -4025,7 +4025,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>149</v>
       </c>
@@ -4033,7 +4033,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -4041,7 +4041,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>154</v>
       </c>
@@ -4049,7 +4049,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>139</v>
       </c>
@@ -4057,7 +4057,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>140</v>
       </c>
@@ -4065,7 +4065,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>141</v>
       </c>
@@ -4073,7 +4073,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>150</v>
       </c>
@@ -4081,7 +4081,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>142</v>
       </c>
@@ -4089,7 +4089,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>29</v>
       </c>
@@ -4100,7 +4100,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>30</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>31</v>
       </c>
@@ -4122,7 +4122,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>32</v>
       </c>
@@ -4133,7 +4133,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>33</v>
       </c>
@@ -4144,7 +4144,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>151</v>
       </c>
@@ -4155,7 +4155,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>34</v>
       </c>
@@ -4166,7 +4166,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>40</v>
       </c>
@@ -4174,7 +4174,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>41</v>
       </c>
@@ -4182,7 +4182,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>42</v>
       </c>
@@ -4190,7 +4190,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>43</v>
       </c>
@@ -4198,7 +4198,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>152</v>
       </c>
@@ -4206,7 +4206,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>44</v>
       </c>
@@ -4214,7 +4214,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>143</v>
       </c>
@@ -4222,7 +4222,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>144</v>
       </c>
@@ -4230,7 +4230,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>145</v>
       </c>
@@ -4238,7 +4238,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>146</v>
       </c>
@@ -4246,7 +4246,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>153</v>
       </c>
@@ -4254,7 +4254,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>147</v>
       </c>
@@ -4262,7 +4262,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>49</v>
       </c>
@@ -4273,7 +4273,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>50</v>
       </c>
@@ -4284,7 +4284,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>51</v>
       </c>
@@ -4295,7 +4295,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>52</v>
       </c>
@@ -4306,7 +4306,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>53</v>
       </c>
@@ -4317,7 +4317,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>162</v>
       </c>
@@ -4328,7 +4328,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>164</v>
       </c>
@@ -4352,17 +4352,17 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="25"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="25"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
         <v>59</v>
       </c>
@@ -4378,7 +4378,7 @@
       <c r="K1" s="19"/>
       <c r="L1" s="19"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4412,7 +4412,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>173</v>
       </c>
@@ -4444,7 +4444,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
         <v>173</v>
       </c>
@@ -4476,7 +4476,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
         <v>173</v>
       </c>
@@ -4508,7 +4508,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
         <v>173</v>
       </c>
@@ -4540,7 +4540,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
         <v>173</v>
       </c>
@@ -4572,7 +4572,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="25" t="s">
         <v>173</v>
       </c>
@@ -4622,14 +4622,14 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.5703125" customWidth="1"/>
-    <col min="3" max="3" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.5546875" customWidth="1"/>
+    <col min="3" max="3" width="49.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>135</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4651,7 +4651,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -4662,7 +4662,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>45</v>
       </c>
@@ -4673,7 +4673,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>46</v>
       </c>
@@ -4684,7 +4684,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>47</v>
       </c>
@@ -4695,7 +4695,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>48</v>
       </c>
@@ -4703,7 +4703,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>123</v>
       </c>
@@ -4714,7 +4714,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>124</v>
       </c>
@@ -4725,7 +4725,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>125</v>
       </c>
@@ -4736,7 +4736,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>158</v>
       </c>
@@ -4753,45 +4753,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
-    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
-    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2020-10-21T13:32:44+00:00</Document_x0020_Creation_x0020_Date>
-    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j747ac98061d40f0aa7bd47e1db5675d>
-    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
-    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Creator>
-    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </EPA_x0020_Contributor>
-    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ed970698-2d60-4bab-a048-d9be527522d9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5266,8 +5229,45 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
+    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
+    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2020-10-21T13:32:44+00:00</Document_x0020_Creation_x0020_Date>
+    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j747ac98061d40f0aa7bd47e1db5675d>
+    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
+    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Creator>
+    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </EPA_x0020_Contributor>
+    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ed970698-2d60-4bab-a048-d9be527522d9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5280,6 +5280,37 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{845EA28A-135D-4CD8-9991-40FEAFECD172}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7114BC5-AD14-42E0-B4DD-783E7B689A85}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="8b03727f-4454-4722-b3e6-018d8dcaf2fd"/>
+    <ds:schemaRef ds:uri="ed970698-2d60-4bab-a048-d9be527522d9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D26D44A-9508-4707-B138-18882E5BA6FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -5288,18 +5319,7 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7114BC5-AD14-42E0-B4DD-783E7B689A85}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{845EA28A-135D-4CD8-9991-40FEAFECD172}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="ed970698-2d60-4bab-a048-d9be527522d9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>